<commit_message>
Added support for parsing node_id as an optional column in input spreadsheets
</commit_message>
<xml_diff>
--- a/src/pds_doi_service/core/input/test/data/spreadsheet_with_optional_columns.xlsx
+++ b/src/pds_doi_service/core/input/test/data/spreadsheet_with_optional_columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinss/repos/pds-doi-service/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinss/repos/pds-doi-service/src/pds_doi_service/core/input/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B33F307C-A86A-5B4F-B18B-6DFE8B5A9763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3525BC7-4429-8E4F-8AD7-861150874CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1980" windowWidth="27300" windowHeight="13660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1980" windowWidth="27300" windowHeight="13660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>title</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>https://pds.nasa.gov/ds-view/pds/viewCollection.jsp?identifier=urn:nasa:pds:lab_shocked_feldspars</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>img</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -409,7 +415,7 @@
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,10 +441,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -464,6 +473,9 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>